<commit_message>
added the hotel supplies
</commit_message>
<xml_diff>
--- a/2017年参展行程.xlsx
+++ b/2017年参展行程.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -132,6 +132,18 @@
   </si>
   <si>
     <t>行业</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>酒店用品</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017/9/8---2017/9/10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第十五届广州国际酒店用品展览会（HOSFAIR）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -288,7 +300,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -301,18 +313,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -320,6 +335,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -602,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:F15"/>
+  <dimension ref="C4:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -622,9 +640,9 @@
       <c r="C4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.15">
       <c r="C5" s="2" t="s">
@@ -641,7 +659,7 @@
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -655,7 +673,7 @@
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C7" s="7"/>
+      <c r="C7" s="5"/>
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
@@ -667,13 +685,13 @@
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -687,7 +705,7 @@
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C10" s="9"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
@@ -699,7 +717,7 @@
       </c>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C11" s="9"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="2" t="s">
         <v>12</v>
       </c>
@@ -711,7 +729,7 @@
       </c>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C12" s="9"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
@@ -723,7 +741,7 @@
       </c>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C13" s="9"/>
+      <c r="C13" s="10"/>
       <c r="D13" s="2" t="s">
         <v>16</v>
       </c>
@@ -735,7 +753,7 @@
       </c>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C14" s="9"/>
+      <c r="C14" s="10"/>
       <c r="D14" s="2" t="s">
         <v>17</v>
       </c>
@@ -747,7 +765,7 @@
       </c>
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.15">
-      <c r="C15" s="10"/>
+      <c r="C15" s="11"/>
       <c r="D15" s="2" t="s">
         <v>19</v>
       </c>
@@ -758,11 +776,33 @@
         <v>6</v>
       </c>
     </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.15">
+      <c r="C16" s="12"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.15">
+      <c r="C17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="C9:C15"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C16:F16"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>